<commit_message>
Update to code to reflect review responses
</commit_message>
<xml_diff>
--- a/v1/MinMax_Key_Features.xlsx
+++ b/v1/MinMax_Key_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mudu605/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mudu605/Desktop/topic_5_scaling/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5B5E1B-6B09-2744-82BF-A2838ED7626F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC124B5-6D22-174F-8734-C947BB922D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="500" windowWidth="35940" windowHeight="23400" xr2:uid="{B28486C3-FA4A-5A44-986D-AB7CFEDB92BA}"/>
+    <workbookView xWindow="66480" yWindow="10080" windowWidth="35940" windowHeight="23400" xr2:uid="{B28486C3-FA4A-5A44-986D-AB7CFEDB92BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Latitude</t>
   </si>
@@ -162,6 +162,57 @@
   </si>
   <si>
     <t>'Mean summer stream temperature - MSST'</t>
+  </si>
+  <si>
+    <t>#   WHONDRS features</t>
+  </si>
+  <si>
+    <t>#       'DS_Water.Column.Height_cm'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#       'SW_Temp_degC'            </t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>#   StreamStats features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#       'lat'     </t>
+  </si>
+  <si>
+    <t>#       'DRNAREA'</t>
+  </si>
+  <si>
+    <t>#   HydroSheds features</t>
+  </si>
+  <si>
+    <t>#       'Natural discharge - dis_m3_pmn'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#       'Air temp - tmp_dc_s05'         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#       'Potential ET - pet_mm_s04'      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#       'Actual ET - aet_mm_s04'        </t>
+  </si>
+  <si>
+    <t>#   EPAW-Catchment features</t>
+  </si>
+  <si>
+    <t>#       'Mean summer stream temperature - MSST'</t>
+  </si>
+  <si>
+    <t>#   EPAW-Watershed features</t>
+  </si>
+  <si>
+    <t>#       'PctImpWs'</t>
+  </si>
+  <si>
+    <t>#       'TmeanWs'</t>
   </si>
 </sst>
 </file>
@@ -540,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE11924-5D33-C344-9BD9-DAB33C241F8A}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,14 +845,114 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>